<commit_message>
excel doc for analysis
</commit_message>
<xml_diff>
--- a/docs/freqs.xlsx
+++ b/docs/freqs.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="chart1" sheetId="4" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="24">
   <si>
     <t>ham</t>
   </si>
@@ -254,72 +255,66 @@
             <c:strRef>
               <c:f>Sheet1!$J$2:$J$23</c:f>
               <c:strCache>
-                <c:ptCount val="22"/>
-                <c:pt idx="0">
+                <c:ptCount val="21"/>
+                <c:pt idx="1">
+                  <c:v>enron</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>gas</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>hpl</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>meter</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>research</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>with</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>for</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>nom</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>and</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>of</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>the</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>in</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>to</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>a</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>actuals</c:v>
-                </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="15">
                   <c:v>all</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>and</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>enron</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>for</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>gas</c:v>
-                </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="16">
                   <c:v>get</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>hpl</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>in</c:v>
-                </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="17">
                   <c:v>is</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>meter</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>nom</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>of</c:v>
-                </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="18">
                   <c:v>on</c:v>
                 </c:pt>
-                <c:pt idx="15">
-                  <c:v>research</c:v>
-                </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="19">
                   <c:v>software</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>the</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>to</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>with</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>your</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>you</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -330,78 +325,72 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
-                <c:pt idx="0">
-                  <c:v>5.1818397908248155</c:v>
-                </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.1630615640599005</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.3023532208224387</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.9662467316377459</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>5.9662467316377459</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.3056810078440697</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.3023532208224387</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.4228666508200618</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.538388400285239</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.9950083194675541</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.5826004278583312</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.1818397908248155</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.1630615640599005</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>2.1155217494651772</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.9950083194675541</c:v>
-                </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="17">
                   <c:v>2.3056810078440697</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2.3056810078440697</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>3.4228666508200618</c:v>
-                </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="18">
                   <c:v>3.375326836225339</c:v>
                 </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="19">
                   <c:v>3.1138578559543615</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>5.538388400285239</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>7.5826004278583312</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>9.103874494889471</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>7.5826004278583312</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4298-4B3E-910A-6C173698139E}"/>
+              <c16:uniqueId val="{00000000-0624-421C-89CF-FCF2ECF57F1D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -433,72 +422,66 @@
             <c:strRef>
               <c:f>Sheet1!$J$2:$J$23</c:f>
               <c:strCache>
-                <c:ptCount val="22"/>
-                <c:pt idx="0">
+                <c:ptCount val="21"/>
+                <c:pt idx="1">
+                  <c:v>enron</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>gas</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>hpl</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>meter</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>research</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>with</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>for</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>nom</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>and</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>of</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>the</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>in</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>to</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>a</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>actuals</c:v>
-                </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="15">
                   <c:v>all</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>and</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>enron</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>for</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>gas</c:v>
-                </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="16">
                   <c:v>get</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>hpl</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>in</c:v>
-                </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="17">
                   <c:v>is</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>meter</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>nom</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>of</c:v>
-                </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="18">
                   <c:v>on</c:v>
                 </c:pt>
-                <c:pt idx="15">
-                  <c:v>research</c:v>
-                </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="19">
                   <c:v>software</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>the</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>to</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>with</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>your</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>you</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -509,70 +492,64 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.3151687233810203</c:v>
+                  <c:v>3.1560554766845037</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2.5226602599104511</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>2.959484547340832</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.5554220814677295</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.7472971497215246</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.6162498634924101</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14.469804521131374</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.1014524407557058</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>4.0952276946598234</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.1560554766845037</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>14.469804521131374</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.5226602599104511</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2.959484547340832</c:v>
-                </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
+                  <c:v>2.8502784754832371</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.0796112263841868</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>1.6162498634924101</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2.5554220814677295</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>3.1014524407557058</c:v>
-                </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.8502784754832371</c:v>
+                  <c:v>3.6911652287867205</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.7472971497215246</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.0796112263841868</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.6911652287867205</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.6162498634924101</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="21">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -580,7 +557,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-4298-4B3E-910A-6C173698139E}"/>
+              <c16:uniqueId val="{00000001-0624-421C-89CF-FCF2ECF57F1D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -772,11 +749,6 @@
       <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -1325,31 +1297,34 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>9524</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>476249</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:to>
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8670192" cy="6293013"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6874D816-961A-4E32-ACCE-C8FB88AE4F64}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34C22FE8-0FDE-47E8-83B2-72E77610CB79}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1362,7 +1337,7 @@
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:absoluteAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1663,10 +1638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V31" sqref="V31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1712,16 +1687,6 @@
       <c r="G2">
         <v>218</v>
       </c>
-      <c r="J2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2">
-        <f>VLOOKUP($J$2:$J$23,$E$2:$F$15,2)</f>
-        <v>5.1818397908248155</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1744,15 +1709,19 @@
       <c r="G3">
         <v>91</v>
       </c>
+      <c r="I3">
+        <f>K3/SUM(K3:L3)</f>
+        <v>0</v>
+      </c>
       <c r="J3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="K3">
         <v>0</v>
       </c>
       <c r="L3">
-        <f t="shared" ref="L3:L23" si="0">VLOOKUP($J$2:$J$23,$A$2:$B$15,2)</f>
-        <v>2.3151687233810203</v>
+        <f>VLOOKUP($J$2:$J$23,$A$2:$B$15,2)</f>
+        <v>3.1560554766845037</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1776,15 +1745,19 @@
       <c r="G4">
         <v>181</v>
       </c>
+      <c r="I4">
+        <f>K4/SUM(K4:L4)</f>
+        <v>0</v>
+      </c>
       <c r="J4" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="K4">
-        <f t="shared" ref="K3:K23" si="1">VLOOKUP($J$2:$J$23,$E$2:$F$15,2)</f>
-        <v>2.1630615640599005</v>
+        <v>0</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <f>VLOOKUP($J$2:$J$23,$A$2:$B$15,2)</f>
+        <v>2.5226602599104511</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1808,16 +1781,19 @@
       <c r="G5">
         <v>251</v>
       </c>
+      <c r="I5">
+        <f>K5/SUM(K5:L5)</f>
+        <v>0</v>
+      </c>
       <c r="J5" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="K5">
-        <f t="shared" si="1"/>
-        <v>4.3023532208224387</v>
+        <v>0</v>
       </c>
       <c r="L5">
-        <f t="shared" si="0"/>
-        <v>4.0952276946598234</v>
+        <f>VLOOKUP($J$2:$J$23,$A$2:$B$15,2)</f>
+        <v>2.959484547340832</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1841,15 +1817,19 @@
       <c r="G6">
         <v>89</v>
       </c>
+      <c r="I6">
+        <f>K6/SUM(K6:L6)</f>
+        <v>0</v>
+      </c>
       <c r="J6" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="K6">
         <v>0</v>
       </c>
       <c r="L6">
-        <f t="shared" si="0"/>
-        <v>3.1560554766845037</v>
+        <f>VLOOKUP($J$2:$J$23,$A$2:$B$15,2)</f>
+        <v>2.5554220814677295</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1873,16 +1853,19 @@
       <c r="G7">
         <v>126</v>
       </c>
+      <c r="I7">
+        <f>K7/SUM(K7:L7)</f>
+        <v>0</v>
+      </c>
       <c r="J7" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="K7">
-        <f t="shared" si="1"/>
-        <v>5.9662467316377459</v>
+        <v>0</v>
       </c>
       <c r="L7">
-        <f t="shared" si="0"/>
-        <v>14.469804521131374</v>
+        <f>VLOOKUP($J$2:$J$23,$A$2:$B$15,2)</f>
+        <v>1.7472971497215246</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1906,15 +1889,19 @@
       <c r="G8">
         <v>97</v>
       </c>
+      <c r="I8">
+        <f>K8/SUM(K8:L8)</f>
+        <v>0</v>
+      </c>
       <c r="J8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="K8">
         <v>0</v>
       </c>
       <c r="L8">
-        <f t="shared" si="0"/>
-        <v>2.5226602599104511</v>
+        <f>VLOOKUP($J$2:$J$23,$A$2:$B$15,2)</f>
+        <v>1.6162498634924101</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1938,15 +1925,20 @@
       <c r="G9">
         <v>144</v>
       </c>
+      <c r="I9">
+        <f>K9/SUM(K9:L9)</f>
+        <v>0.29194714075838452</v>
+      </c>
       <c r="J9" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="K9">
-        <f t="shared" si="1"/>
-        <v>2.1155217494651772</v>
+        <f>VLOOKUP($J$2:$J$23,$E$2:$F$15,2)</f>
+        <v>5.9662467316377459</v>
       </c>
       <c r="L9">
-        <v>0</v>
+        <f>VLOOKUP($J$2:$J$23,$A$2:$B$15,2)</f>
+        <v>14.469804521131374</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1970,15 +1962,20 @@
       <c r="G10">
         <v>142</v>
       </c>
+      <c r="I10">
+        <f>K10/SUM(K10:L10)</f>
+        <v>0.42641466680300738</v>
+      </c>
       <c r="J10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K10">
-        <v>0</v>
+        <f>VLOOKUP($J$2:$J$23,$E$2:$F$15,2)</f>
+        <v>2.3056810078440697</v>
       </c>
       <c r="L10">
-        <f t="shared" si="0"/>
-        <v>2.959484547340832</v>
+        <f>VLOOKUP($J$2:$J$23,$A$2:$B$15,2)</f>
+        <v>3.1014524407557058</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2002,16 +1999,20 @@
       <c r="G11">
         <v>131</v>
       </c>
+      <c r="I11">
+        <f>K11/SUM(K11:L11)</f>
+        <v>0.51233245194343691</v>
+      </c>
       <c r="J11" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="K11">
-        <f t="shared" si="1"/>
-        <v>2.9950083194675541</v>
+        <f>VLOOKUP($J$2:$J$23,$E$2:$F$15,2)</f>
+        <v>4.3023532208224387</v>
       </c>
       <c r="L11">
-        <f t="shared" si="0"/>
-        <v>1.6162498634924101</v>
+        <f>VLOOKUP($J$2:$J$23,$A$2:$B$15,2)</f>
+        <v>4.0952276946598234</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -2035,15 +2036,20 @@
       <c r="G12">
         <v>233</v>
       </c>
+      <c r="I12">
+        <f>K12/SUM(K12:L12)</f>
+        <v>0.54563804629164103</v>
+      </c>
       <c r="J12" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="K12">
-        <f t="shared" si="1"/>
-        <v>2.3056810078440697</v>
+        <f>VLOOKUP($J$2:$J$23,$E$2:$F$15,2)</f>
+        <v>3.4228666508200618</v>
       </c>
       <c r="L12">
-        <v>0</v>
+        <f>VLOOKUP($J$2:$J$23,$A$2:$B$15,2)</f>
+        <v>2.8502784754832371</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -2067,15 +2073,20 @@
       <c r="G13">
         <v>319</v>
       </c>
+      <c r="I13">
+        <f>K13/SUM(K13:L13)</f>
+        <v>0.6426535901842042</v>
+      </c>
       <c r="J13" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="K13">
-        <v>0</v>
+        <f>VLOOKUP($J$2:$J$23,$E$2:$F$15,2)</f>
+        <v>5.538388400285239</v>
       </c>
       <c r="L13">
-        <f t="shared" si="0"/>
-        <v>2.5554220814677295</v>
+        <f>VLOOKUP($J$2:$J$23,$A$2:$B$15,2)</f>
+        <v>3.0796112263841868</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2099,16 +2110,20 @@
       <c r="G14">
         <v>383</v>
       </c>
+      <c r="I14">
+        <f>K14/SUM(K14:L14)</f>
+        <v>0.64949916067051794</v>
+      </c>
       <c r="J14" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="K14">
-        <f t="shared" si="1"/>
-        <v>2.3056810078440697</v>
+        <f>VLOOKUP($J$2:$J$23,$E$2:$F$15,2)</f>
+        <v>2.9950083194675541</v>
       </c>
       <c r="L14">
-        <f t="shared" si="0"/>
-        <v>3.1014524407557058</v>
+        <f>VLOOKUP($J$2:$J$23,$A$2:$B$15,2)</f>
+        <v>1.6162498634924101</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -2132,121 +2147,138 @@
       <c r="G15">
         <v>239</v>
       </c>
+      <c r="I15">
+        <f>K15/SUM(K15:L15)</f>
+        <v>0.67258808270410941</v>
+      </c>
       <c r="J15" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="K15">
-        <f t="shared" si="1"/>
-        <v>3.4228666508200618</v>
+        <f>VLOOKUP($J$2:$J$23,$E$2:$F$15,2)</f>
+        <v>7.5826004278583312</v>
       </c>
       <c r="L15">
-        <f t="shared" si="0"/>
-        <v>2.8502784754832371</v>
+        <f>VLOOKUP($J$2:$J$23,$A$2:$B$15,2)</f>
+        <v>3.6911652287867205</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <f>K16/SUM(K16:L16)</f>
+        <v>1</v>
+      </c>
       <c r="J16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K16">
-        <f t="shared" si="1"/>
-        <v>3.375326836225339</v>
+        <f>VLOOKUP($J$2:$J$23,$E$2:$F$15,2)</f>
+        <v>5.1818397908248155</v>
       </c>
       <c r="L16">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="10:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <f>K17/SUM(K17:L17)</f>
+        <v>1</v>
+      </c>
       <c r="J17" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="K17">
+        <f>VLOOKUP($J$2:$J$23,$E$2:$F$15,2)</f>
+        <v>2.1630615640599005</v>
+      </c>
+      <c r="L17">
         <v>0</v>
       </c>
-      <c r="L17">
-        <f t="shared" si="0"/>
-        <v>1.7472971497215246</v>
-      </c>
     </row>
-    <row r="18" spans="10:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <f>K18/SUM(K18:L18)</f>
+        <v>1</v>
+      </c>
       <c r="J18" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="K18">
-        <f t="shared" si="1"/>
-        <v>3.1138578559543615</v>
+        <f>VLOOKUP($J$2:$J$23,$E$2:$F$15,2)</f>
+        <v>2.1155217494651772</v>
       </c>
       <c r="L18">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="10:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <f>K19/SUM(K19:L19)</f>
+        <v>1</v>
+      </c>
       <c r="J19" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="K19">
-        <f t="shared" si="1"/>
-        <v>5.538388400285239</v>
+        <f>VLOOKUP($J$2:$J$23,$E$2:$F$15,2)</f>
+        <v>2.3056810078440697</v>
       </c>
       <c r="L19">
-        <f t="shared" si="0"/>
-        <v>3.0796112263841868</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="20" spans="10:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <f>K20/SUM(K20:L20)</f>
+        <v>1</v>
+      </c>
       <c r="J20" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="K20">
-        <f t="shared" si="1"/>
-        <v>7.5826004278583312</v>
+        <f>VLOOKUP($J$2:$J$23,$E$2:$F$15,2)</f>
+        <v>3.375326836225339</v>
       </c>
       <c r="L20">
-        <f t="shared" si="0"/>
-        <v>3.6911652287867205</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="21" spans="10:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <f>K21/SUM(K21:L21)</f>
+        <v>1</v>
+      </c>
       <c r="J21" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="K21">
+        <f>VLOOKUP($J$2:$J$23,$E$2:$F$15,2)</f>
+        <v>3.1138578559543615</v>
+      </c>
+      <c r="L21">
         <v>0</v>
       </c>
-      <c r="L21">
-        <f t="shared" si="0"/>
-        <v>1.6162498634924101</v>
-      </c>
     </row>
-    <row r="22" spans="10:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="I22">
+        <f>K22/SUM(K22:L22)</f>
+        <v>1</v>
+      </c>
       <c r="J22" t="s">
         <v>16</v>
       </c>
       <c r="K22">
-        <f t="shared" si="1"/>
+        <f>VLOOKUP($J$2:$J$23,$E$2:$F$15,2)</f>
         <v>9.103874494889471</v>
       </c>
       <c r="L22">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="J23" t="s">
-        <v>23</v>
-      </c>
-      <c r="K23">
-        <f t="shared" si="1"/>
-        <v>7.5826004278583312</v>
-      </c>
-      <c r="L23">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState ref="J2:J29">
-    <sortCondition ref="J2"/>
+  <sortState ref="I2:L23">
+    <sortCondition ref="I2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>